<commit_message>
Read last empty cell of a row
</commit_message>
<xml_diff>
--- a/tests/Data.Xls.Tests/Sources/emptyCells.xlsx
+++ b/tests/Data.Xls.Tests/Sources/emptyCells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\FileBasedDataProvider\tests\Data.Xls.Tests\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC5BA1-51DB-4871-80CB-561997379865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1194DE0-1248-4A15-A063-2AE552362F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{25EDF2C7-5250-40E1-9A28-C813ADF7E7C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Carl</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
   </si>
 </sst>
 </file>
@@ -95,8 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,15 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F59143D-CFF9-4B6F-85FE-D020A68354C5}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +459,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,8 +473,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="1">
+        <v>34100.11037037037</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>20</v>
       </c>
@@ -472,12 +485,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>34100.11037037037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>